<commit_message>
Push with updated Mishustin data
</commit_message>
<xml_diff>
--- a/raw-data/mishustin.xlsx
+++ b/raw-data/mishustin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshap\Documents\GOV-1006\levadasept\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA24BE4-729F-49C8-AECA-029F31E13B11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF865D34-D319-499F-A7DF-F74B9771C82C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5BCEB3FA-7AE5-4D8E-913E-5BACF3314482}"/>
   </bookViews>
@@ -415,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E7DDA8-2F64-4FDA-A6D7-F99B28609814}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -444,7 +444,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -455,7 +455,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -466,7 +466,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>